<commit_message>
Alternate model and results
This model uses

mu.fecundity
mu.fl.per.head
mu.seed.mass
mu.infest

instead of observed means as covariates in pink and poly regressions.

DIC indistinguishable, but Dhat is worse.
</commit_message>
<xml_diff>
--- a/DIC-results.xlsx
+++ b/DIC-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="260" windowWidth="29600" windowHeight="18240" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="-20" windowWidth="29600" windowHeight="18340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,38 +19,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Model</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Dbar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Dhat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>DIC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Full</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full-alt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -93,10 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -427,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -461,22 +477,40 @@
       </c>
       <c r="B2" s="2">
         <f>E2-D2</f>
-        <v>209.91700000000003</v>
+        <v>212.18799999999999</v>
       </c>
       <c r="C2" s="2">
         <f>B2-D2</f>
-        <v>111.42600000000003</v>
+        <v>131.363</v>
       </c>
       <c r="D2" s="2">
-        <v>98.491</v>
+        <v>80.825000000000003</v>
       </c>
       <c r="E2" s="2">
-        <v>308.40800000000002</v>
+        <v>293.01299999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <f>E3-D3</f>
+        <v>223.56400000000002</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3-D3</f>
+        <v>153.39300000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>70.171000000000006</v>
+      </c>
+      <c r="E3" s="2">
+        <v>293.73500000000001</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Preliminary changes for plotting
* Model choice for separete slopes vs. common slopes (repens vs.
whites): *-no-repens.txt, DIC-results.xlsx, models.txt
* updated ..gitignore, to-do.txt
* deleted results-full-alt.txt
* plot-results.R: does not do proper averaging yet
</commit_message>
<xml_diff>
--- a/DIC-results.xlsx
+++ b/DIC-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="-20" windowWidth="29600" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="-20" windowWidth="29600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Full-alt</t>
+    <t>No-repens</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -477,17 +477,17 @@
       </c>
       <c r="B2" s="2">
         <f>E2-D2</f>
-        <v>212.18799999999999</v>
+        <v>212.3</v>
       </c>
       <c r="C2" s="2">
         <f>B2-D2</f>
-        <v>131.363</v>
+        <v>78.600000000000023</v>
       </c>
       <c r="D2" s="2">
-        <v>80.825000000000003</v>
+        <v>133.69999999999999</v>
       </c>
       <c r="E2" s="2">
-        <v>293.01299999999998</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -496,17 +496,17 @@
       </c>
       <c r="B3" s="2">
         <f>E3-D3</f>
-        <v>223.56400000000002</v>
+        <v>221.5</v>
       </c>
       <c r="C3" s="2">
         <f>B3-D3</f>
-        <v>153.39300000000003</v>
+        <v>128.80000000000001</v>
       </c>
       <c r="D3" s="2">
-        <v>70.171000000000006</v>
+        <v>92.7</v>
       </c>
       <c r="E3" s="2">
-        <v>293.73500000000001</v>
+        <v>314.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>